<commit_message>
fix method writeExcel. Add method ReadExcel
</commit_message>
<xml_diff>
--- a/demoApachePOI/excelEx.xlsx
+++ b/demoApachePOI/excelEx.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -35,307 +35,172 @@
     <t>TOTAL MONEY</t>
   </si>
   <si>
-    <t>firstName1</t>
-  </si>
-  <si>
-    <t>lastName1</t>
-  </si>
-  <si>
-    <t>Hue</t>
-  </si>
-  <si>
-    <t>firstName2</t>
-  </si>
-  <si>
-    <t>lastName2</t>
-  </si>
-  <si>
-    <t>firstName3</t>
-  </si>
-  <si>
-    <t>lastName3</t>
-  </si>
-  <si>
-    <t>firstName4</t>
-  </si>
-  <si>
-    <t>lastName4</t>
-  </si>
-  <si>
-    <t>firstName5</t>
-  </si>
-  <si>
-    <t>lastName5</t>
-  </si>
-  <si>
-    <t>firstName6</t>
-  </si>
-  <si>
-    <t>lastName6</t>
-  </si>
-  <si>
-    <t>firstName7</t>
-  </si>
-  <si>
-    <t>lastName7</t>
-  </si>
-  <si>
-    <t>firstName8</t>
-  </si>
-  <si>
-    <t>lastName8</t>
-  </si>
-  <si>
-    <t>firstName9</t>
-  </si>
-  <si>
-    <t>lastName9</t>
-  </si>
-  <si>
-    <t>firstName10</t>
-  </si>
-  <si>
-    <t>lastName10</t>
-  </si>
-  <si>
-    <t>firstName11</t>
-  </si>
-  <si>
-    <t>lastName11</t>
-  </si>
-  <si>
-    <t>firstName12</t>
-  </si>
-  <si>
-    <t>lastName12</t>
-  </si>
-  <si>
-    <t>firstName13</t>
-  </si>
-  <si>
-    <t>lastName13</t>
-  </si>
-  <si>
-    <t>firstName14</t>
-  </si>
-  <si>
-    <t>lastName14</t>
-  </si>
-  <si>
-    <t>firstName15</t>
-  </si>
-  <si>
-    <t>lastName15</t>
-  </si>
-  <si>
-    <t>firstName16</t>
-  </si>
-  <si>
-    <t>lastName16</t>
-  </si>
-  <si>
-    <t>firstName17</t>
-  </si>
-  <si>
-    <t>lastName17</t>
-  </si>
-  <si>
-    <t>firstName18</t>
-  </si>
-  <si>
-    <t>lastName18</t>
-  </si>
-  <si>
-    <t>firstName19</t>
-  </si>
-  <si>
-    <t>lastName19</t>
-  </si>
-  <si>
-    <t>firstName20</t>
-  </si>
-  <si>
-    <t>lastName20</t>
-  </si>
-  <si>
-    <t>firstName21</t>
-  </si>
-  <si>
-    <t>lastName21</t>
-  </si>
-  <si>
-    <t>firstName22</t>
-  </si>
-  <si>
-    <t>lastName22</t>
-  </si>
-  <si>
-    <t>firstName23</t>
-  </si>
-  <si>
-    <t>lastName23</t>
-  </si>
-  <si>
-    <t>firstName24</t>
-  </si>
-  <si>
-    <t>lastName24</t>
-  </si>
-  <si>
-    <t>firstName25</t>
-  </si>
-  <si>
-    <t>lastName25</t>
-  </si>
-  <si>
-    <t>firstName26</t>
-  </si>
-  <si>
-    <t>lastName26</t>
-  </si>
-  <si>
-    <t>firstName27</t>
-  </si>
-  <si>
-    <t>lastName27</t>
-  </si>
-  <si>
-    <t>firstName28</t>
-  </si>
-  <si>
-    <t>lastName28</t>
-  </si>
-  <si>
-    <t>firstName29</t>
-  </si>
-  <si>
-    <t>lastName29</t>
-  </si>
-  <si>
-    <t>firstName30</t>
-  </si>
-  <si>
-    <t>lastName30</t>
-  </si>
-  <si>
-    <t>firstName31</t>
-  </si>
-  <si>
-    <t>lastName31</t>
-  </si>
-  <si>
-    <t>firstName32</t>
-  </si>
-  <si>
-    <t>lastName32</t>
-  </si>
-  <si>
-    <t>firstName33</t>
-  </si>
-  <si>
-    <t>lastName33</t>
-  </si>
-  <si>
-    <t>firstName34</t>
-  </si>
-  <si>
-    <t>lastName34</t>
-  </si>
-  <si>
-    <t>firstName35</t>
-  </si>
-  <si>
-    <t>lastName35</t>
-  </si>
-  <si>
-    <t>firstName36</t>
-  </si>
-  <si>
-    <t>lastName36</t>
-  </si>
-  <si>
-    <t>firstName37</t>
-  </si>
-  <si>
-    <t>lastName37</t>
-  </si>
-  <si>
-    <t>firstName38</t>
-  </si>
-  <si>
-    <t>lastName38</t>
-  </si>
-  <si>
-    <t>firstName39</t>
-  </si>
-  <si>
-    <t>lastName39</t>
-  </si>
-  <si>
-    <t>firstName40</t>
-  </si>
-  <si>
-    <t>lastName40</t>
-  </si>
-  <si>
-    <t>firstName41</t>
-  </si>
-  <si>
-    <t>lastName41</t>
-  </si>
-  <si>
-    <t>firstName42</t>
-  </si>
-  <si>
-    <t>lastName42</t>
-  </si>
-  <si>
-    <t>firstName43</t>
-  </si>
-  <si>
-    <t>lastName43</t>
-  </si>
-  <si>
-    <t>firstName44</t>
-  </si>
-  <si>
-    <t>lastName44</t>
-  </si>
-  <si>
-    <t>firstName45</t>
-  </si>
-  <si>
-    <t>lastName45</t>
-  </si>
-  <si>
-    <t>firstName46</t>
-  </si>
-  <si>
-    <t>lastName46</t>
-  </si>
-  <si>
-    <t>firstName47</t>
-  </si>
-  <si>
-    <t>lastName47</t>
-  </si>
-  <si>
-    <t>firstName48</t>
-  </si>
-  <si>
-    <t>lastName48</t>
-  </si>
-  <si>
-    <t>firstName49</t>
-  </si>
-  <si>
-    <t>lastName49</t>
-  </si>
-  <si>
-    <t>firstName50</t>
-  </si>
-  <si>
-    <t>lastName50</t>
+    <t/>
+  </si>
+  <si>
+    <t>Tứ</t>
+  </si>
+  <si>
+    <t>Lê Nhã</t>
+  </si>
+  <si>
+    <t>Quảng Nam</t>
+  </si>
+  <si>
+    <t>Lan</t>
+  </si>
+  <si>
+    <t>Trần Huỳnh</t>
+  </si>
+  <si>
+    <t>Đà Nẵng</t>
+  </si>
+  <si>
+    <t>Huệ</t>
+  </si>
+  <si>
+    <t>Nguyễn Công</t>
+  </si>
+  <si>
+    <t>Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Hoa</t>
+  </si>
+  <si>
+    <t>Huỳnh Như</t>
+  </si>
+  <si>
+    <t>Đồng Nai</t>
+  </si>
+  <si>
+    <t>Lộc</t>
+  </si>
+  <si>
+    <t>Hoàng Nhã</t>
+  </si>
+  <si>
+    <t>Huyền</t>
+  </si>
+  <si>
+    <t>Nguyễn Gia</t>
+  </si>
+  <si>
+    <t>Phạm Ngọc</t>
+  </si>
+  <si>
+    <t>Hải Dương</t>
+  </si>
+  <si>
+    <t>Hổ</t>
+  </si>
+  <si>
+    <t>Hoàng Văn</t>
+  </si>
+  <si>
+    <t>Phạm Văn</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>Nhị</t>
+  </si>
+  <si>
+    <t>Đào Như</t>
+  </si>
+  <si>
+    <t>Phạm Như</t>
+  </si>
+  <si>
+    <t>Quảng Ninh</t>
+  </si>
+  <si>
+    <t>Lê Công</t>
+  </si>
+  <si>
+    <t>Lê Văn</t>
+  </si>
+  <si>
+    <t>Vũng Tàu</t>
+  </si>
+  <si>
+    <t>Tam</t>
+  </si>
+  <si>
+    <t>Trần Văn</t>
+  </si>
+  <si>
+    <t>Đào Nhã</t>
+  </si>
+  <si>
+    <t>Ngũ</t>
+  </si>
+  <si>
+    <t>Đào Văn</t>
+  </si>
+  <si>
+    <t>Trần Công</t>
+  </si>
+  <si>
+    <t>Nguyễn Nhã</t>
+  </si>
+  <si>
+    <t>Huế</t>
+  </si>
+  <si>
+    <t>Lê Huỳnh</t>
+  </si>
+  <si>
+    <t>Trần Ngọc</t>
+  </si>
+  <si>
+    <t>Nguyễn Huỳnh</t>
+  </si>
+  <si>
+    <t>Huỳnh Huỳnh</t>
+  </si>
+  <si>
+    <t>Huỳnh Nhã</t>
+  </si>
+  <si>
+    <t>Đào Huỳnh</t>
+  </si>
+  <si>
+    <t>Huỳnh Gia</t>
+  </si>
+  <si>
+    <t>Lê Ngọc</t>
+  </si>
+  <si>
+    <t>Hoàng Như</t>
+  </si>
+  <si>
+    <t>Huỳnh Văn</t>
+  </si>
+  <si>
+    <t>Cúc</t>
+  </si>
+  <si>
+    <t>Phạm Gia</t>
+  </si>
+  <si>
+    <t>Hoàng Công</t>
+  </si>
+  <si>
+    <t>Hoàng Gia</t>
+  </si>
+  <si>
+    <t>Nguyễn Ngọc</t>
+  </si>
+  <si>
+    <t>Đào Ngọc</t>
+  </si>
+  <si>
+    <t>Lê Gia</t>
+  </si>
+  <si>
+    <t>Phạm Công</t>
   </si>
 </sst>
 </file>
@@ -670,8 +535,8 @@
   <cols>
     <col min="1" max="1" width="4.4140625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="16.5390625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="15.2578125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.97265625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="16.85546875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.03515625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="11.69140625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="16.7109375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="18.8671875" customWidth="true" bestFit="true"/>
@@ -705,13 +570,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>500000.0</v>
@@ -728,13 +593,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>1000000.0</v>
@@ -751,13 +616,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>1500000.0</v>
@@ -774,13 +639,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>2000000.0</v>
@@ -797,13 +662,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E6" s="6" t="n">
         <v>2500000.0</v>
@@ -820,13 +685,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E7" s="7" t="n">
         <v>3000000.0</v>
@@ -843,13 +708,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E8" s="8" t="n">
         <v>3500000.0</v>
@@ -866,13 +731,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E9" s="9" t="n">
         <v>4000000.0</v>
@@ -889,13 +754,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E10" s="10" t="n">
         <v>4500000.0</v>
@@ -912,13 +777,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E11" s="11" t="n">
         <v>5000000.0</v>
@@ -935,13 +800,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E12" s="12" t="n">
         <v>5500000.0</v>
@@ -958,13 +823,13 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E13" s="13" t="n">
         <v>6000000.0</v>
@@ -981,13 +846,13 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E14" s="14" t="n">
         <v>6500000.0</v>
@@ -1004,13 +869,13 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E15" s="15" t="n">
         <v>7000000.0</v>
@@ -1027,13 +892,13 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>36</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>9</v>
       </c>
       <c r="E16" s="16" t="n">
         <v>7500000.0</v>
@@ -1050,13 +915,13 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E17" s="17" t="n">
         <v>8000000.0</v>
@@ -1079,7 +944,7 @@
         <v>41</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E18" s="18" t="n">
         <v>8500000.0</v>
@@ -1096,13 +961,13 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>43</v>
-      </c>
       <c r="D19" s="19" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E19" s="19" t="n">
         <v>9000000.0</v>
@@ -1119,13 +984,13 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="20" t="s">
         <v>44</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>9</v>
       </c>
       <c r="E20" s="20" t="n">
         <v>9500000.0</v>
@@ -1142,13 +1007,13 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E21" s="21" t="n">
         <v>1.0E7</v>
@@ -1165,13 +1030,13 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E22" s="22" t="n">
         <v>1.05E7</v>
@@ -1188,13 +1053,13 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E23" s="23" t="n">
         <v>1.1E7</v>
@@ -1211,13 +1076,13 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E24" s="24" t="n">
         <v>1.15E7</v>
@@ -1234,13 +1099,13 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E25" s="25" t="n">
         <v>1.2E7</v>
@@ -1257,13 +1122,13 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E26" s="26" t="n">
         <v>1.25E7</v>
@@ -1280,13 +1145,13 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E27" s="27" t="n">
         <v>1.3E7</v>
@@ -1303,13 +1168,13 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E28" s="28" t="n">
         <v>1.35E7</v>
@@ -1326,13 +1191,13 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E29" s="29" t="n">
         <v>1.4E7</v>
@@ -1349,13 +1214,13 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E30" s="30" t="n">
         <v>1.45E7</v>
@@ -1372,13 +1237,13 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E31" s="31" t="n">
         <v>1.5E7</v>
@@ -1395,13 +1260,13 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E32" s="32" t="n">
         <v>1.55E7</v>
@@ -1418,13 +1283,13 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E33" s="33" t="n">
         <v>1.6E7</v>
@@ -1441,13 +1306,13 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E34" s="34" t="n">
         <v>1.65E7</v>
@@ -1464,13 +1329,13 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="35" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E35" s="35" t="n">
         <v>1.7E7</v>
@@ -1487,13 +1352,13 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E36" s="36" t="n">
         <v>1.75E7</v>
@@ -1510,13 +1375,13 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E37" s="37" t="n">
         <v>1.8E7</v>
@@ -1533,13 +1398,13 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E38" s="38" t="n">
         <v>1.85E7</v>
@@ -1556,13 +1421,13 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E39" s="39" t="n">
         <v>1.9E7</v>
@@ -1579,13 +1444,13 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="40" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E40" s="40" t="n">
         <v>1.95E7</v>
@@ -1602,13 +1467,13 @@
         <v>40.0</v>
       </c>
       <c r="B41" s="41" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="C41" s="41" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="D41" s="41" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E41" s="41" t="n">
         <v>2.0E7</v>
@@ -1625,13 +1490,13 @@
         <v>41.0</v>
       </c>
       <c r="B42" s="42" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C42" s="42" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="D42" s="42" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E42" s="42" t="n">
         <v>2.05E7</v>
@@ -1648,13 +1513,13 @@
         <v>42.0</v>
       </c>
       <c r="B43" s="43" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="C43" s="43" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="D43" s="43" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E43" s="43" t="n">
         <v>2.1E7</v>
@@ -1671,13 +1536,13 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="44" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="D44" s="44" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E44" s="44" t="n">
         <v>2.15E7</v>
@@ -1694,13 +1559,13 @@
         <v>44.0</v>
       </c>
       <c r="B45" s="45" t="s">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="C45" s="45" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="D45" s="45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E45" s="45" t="n">
         <v>2.2E7</v>
@@ -1717,13 +1582,13 @@
         <v>45.0</v>
       </c>
       <c r="B46" s="46" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="C46" s="46" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="D46" s="46" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E46" s="46" t="n">
         <v>2.25E7</v>
@@ -1740,13 +1605,13 @@
         <v>46.0</v>
       </c>
       <c r="B47" s="47" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="C47" s="47" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D47" s="47" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E47" s="47" t="n">
         <v>2.3E7</v>
@@ -1763,13 +1628,13 @@
         <v>47.0</v>
       </c>
       <c r="B48" s="48" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E48" s="48" t="n">
         <v>2.35E7</v>
@@ -1786,13 +1651,13 @@
         <v>48.0</v>
       </c>
       <c r="B49" s="49" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="C49" s="49" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="D49" s="49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E49" s="49" t="n">
         <v>2.4E7</v>
@@ -1809,13 +1674,13 @@
         <v>49.0</v>
       </c>
       <c r="B50" s="50" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="C50" s="50" t="s">
-        <v>105</v>
+        <v>62</v>
       </c>
       <c r="D50" s="50" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E50" s="50" t="n">
         <v>2.45E7</v>
@@ -1832,13 +1697,13 @@
         <v>50.0</v>
       </c>
       <c r="B51" s="51" t="s">
-        <v>106</v>
+        <v>37</v>
       </c>
       <c r="C51" s="51" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="D51" s="51" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E51" s="51" t="n">
         <v>2.5E7</v>

</xml_diff>